<commit_message>
Se completan los datos de las coordenadas sobre el archivo de excel
</commit_message>
<xml_diff>
--- a/service/Resources/Base-jornada-unica.xlsx
+++ b/service/Resources/Base-jornada-unica.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="117">
   <si>
     <t>DEPARTAMENTO</t>
   </si>
@@ -351,6 +351,30 @@
   </si>
   <si>
     <t>ZIPAQUIRÁ</t>
+  </si>
+  <si>
+    <t> -77.002012</t>
+  </si>
+  <si>
+    <t> -75.278077</t>
+  </si>
+  <si>
+    <t>0.744944</t>
+  </si>
+  <si>
+    <t> -71.741300</t>
+  </si>
+  <si>
+    <t> -76.802320</t>
+  </si>
+  <si>
+    <t>0.539869</t>
+  </si>
+  <si>
+    <t>0.648608</t>
+  </si>
+  <si>
+    <t>0.605825</t>
   </si>
 </sst>
 </file>
@@ -420,7 +444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -443,17 +467,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -464,7 +477,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -476,12 +489,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -771,15 +787,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.75" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -811,10 +827,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1161,6 +1177,12 @@
       <c r="I11" s="3">
         <v>24735</v>
       </c>
+      <c r="J11" s="8">
+        <v>4651706</v>
+      </c>
+      <c r="K11" s="8">
+        <v>-74094083</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1190,6 +1212,12 @@
       <c r="I12" s="3">
         <v>0</v>
       </c>
+      <c r="J12" s="8">
+        <v>9175307</v>
+      </c>
+      <c r="K12" s="8">
+        <v>-74629976</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1219,6 +1247,12 @@
       <c r="I13" s="3">
         <v>2974</v>
       </c>
+      <c r="J13" s="8">
+        <v>5603707</v>
+      </c>
+      <c r="K13" s="8">
+        <v>-73177345</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1248,6 +1282,12 @@
       <c r="I14" s="3">
         <v>0</v>
       </c>
+      <c r="J14" s="8">
+        <v>7165358</v>
+      </c>
+      <c r="K14" s="8">
+        <v>-73110994</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -1277,6 +1317,12 @@
       <c r="I15" s="3">
         <v>0</v>
       </c>
+      <c r="J15" s="8">
+        <v>3671854</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1306,8 +1352,14 @@
       <c r="I16" s="3">
         <v>1764</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="8">
+        <v>3899271</v>
+      </c>
+      <c r="K16" s="8">
+        <v>-76298704</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1335,8 +1387,14 @@
       <c r="I17" s="3">
         <v>3095</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="8">
+        <v>5323986</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1364,8 +1422,14 @@
       <c r="I18" s="3">
         <v>4139</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="8">
+        <v>3450924</v>
+      </c>
+      <c r="K18" s="8">
+        <v>-76522576</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
@@ -1393,8 +1457,14 @@
       <c r="I19" s="3">
         <v>1702</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J19" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="8">
+        <v>-74006858</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1422,8 +1492,14 @@
       <c r="I20" s="3">
         <v>834</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="8">
+        <v>10391399</v>
+      </c>
+      <c r="K20" s="8">
+        <v>-75489371</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -1451,8 +1527,14 @@
       <c r="I21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="8">
+        <v>4723677</v>
+      </c>
+      <c r="K21" s="8">
+        <v>-75923086</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -1480,8 +1562,14 @@
       <c r="I22" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="8">
+        <v>5486887</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
@@ -1509,8 +1597,14 @@
       <c r="I23" s="3">
         <v>280</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="8">
+        <v>2364316</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -1538,8 +1632,14 @@
       <c r="I24" s="3">
         <v>2203</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="10">
+        <v>9595171</v>
+      </c>
+      <c r="K24" s="10">
+        <v>-73552219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
@@ -1567,8 +1667,14 @@
       <c r="I25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="10">
+        <v>4863390</v>
+      </c>
+      <c r="K25" s="10">
+        <v>-74052034</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
@@ -1596,8 +1702,14 @@
       <c r="I26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="10">
+        <v>5146402</v>
+      </c>
+      <c r="K26" s="10">
+        <v>-73683013</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>41</v>
       </c>
@@ -1625,12 +1737,18 @@
       <c r="I27" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="10">
+        <v>11008298</v>
+      </c>
+      <c r="K27" s="10">
+        <v>-74246374</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C28" s="3">
@@ -1654,8 +1772,14 @@
       <c r="I28" s="3">
         <v>318</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="10">
+        <v>8439250</v>
+      </c>
+      <c r="K28" s="10">
+        <v>-75853045</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
@@ -1683,8 +1807,14 @@
       <c r="I29" s="3">
         <v>9992</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J29" s="10">
+        <v>8141635</v>
+      </c>
+      <c r="K29" s="10">
+        <v>-72466244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -1712,8 +1842,14 @@
       <c r="I30" s="3">
         <v>8037</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J30" s="10">
+        <v>5220047</v>
+      </c>
+      <c r="K30" s="10">
+        <v>-74182339</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>46</v>
       </c>
@@ -1741,8 +1877,14 @@
       <c r="I31" s="3">
         <v>1868</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="10">
+        <v>4830768</v>
+      </c>
+      <c r="K31" s="10">
+        <v>-75680123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>25</v>
       </c>
@@ -1770,8 +1912,14 @@
       <c r="I32" s="3">
         <v>1472</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="10">
+        <v>5890628</v>
+      </c>
+      <c r="K32" s="10">
+        <v>-73063855</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>10</v>
       </c>
@@ -1799,8 +1947,14 @@
       <c r="I33" s="3">
         <v>7808</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J33" s="10">
+        <v>6168616</v>
+      </c>
+      <c r="K33" s="10">
+        <v>-75587079</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
@@ -1828,8 +1982,14 @@
       <c r="I34" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="10">
+        <v>4842440</v>
+      </c>
+      <c r="K34" s="10">
+        <v>-74344428</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>32</v>
       </c>
@@ -1857,8 +2017,14 @@
       <c r="I35" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J35" s="10">
+        <v>1763731</v>
+      </c>
+      <c r="K35" s="10">
+        <v>-75570294</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>18</v>
       </c>
@@ -1886,8 +2052,14 @@
       <c r="I36" s="3">
         <v>1012</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J36" s="10">
+        <v>7071031</v>
+      </c>
+      <c r="K36" s="10">
+        <v>-73106217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
@@ -1915,8 +2087,14 @@
       <c r="I37" s="3">
         <v>2587</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="10">
+        <v>4319713</v>
+      </c>
+      <c r="K37" s="10">
+        <v>-74402246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>38</v>
       </c>
@@ -1944,8 +2122,14 @@
       <c r="I38" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="10">
+        <v>4303349</v>
+      </c>
+      <c r="K38" s="10">
+        <v>-74803123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>18</v>
       </c>
@@ -1973,12 +2157,18 @@
       <c r="I39" s="3">
         <v>2349</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="10">
+        <v>7073129</v>
+      </c>
+      <c r="K39" s="10">
+        <v>-73169203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C40" s="3">
@@ -2002,8 +2192,14 @@
       <c r="I40" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="10">
+        <v>2971477</v>
+      </c>
+      <c r="K40" s="10">
+        <v>-68969510</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>57</v>
       </c>
@@ -2031,8 +2227,14 @@
       <c r="I41" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="10">
+        <v>2095879</v>
+      </c>
+      <c r="K41" s="10">
+        <v>72249173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>58</v>
       </c>
@@ -2060,8 +2262,14 @@
       <c r="I42" s="3">
         <v>2542</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="10">
+        <v>2749019</v>
+      </c>
+      <c r="K42" s="10">
+        <v>-75449037</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>59</v>
       </c>
@@ -2089,8 +2297,14 @@
       <c r="I43" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="10">
+        <v>4441213</v>
+      </c>
+      <c r="K43" s="10">
+        <v>-75238791</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>61</v>
       </c>
@@ -2118,8 +2332,14 @@
       <c r="I44" s="3">
         <v>586</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K44" s="10">
+        <v>-77439853</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>10</v>
       </c>
@@ -2147,8 +2367,14 @@
       <c r="I45" s="3">
         <v>4329</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="10">
+        <v>6169447</v>
+      </c>
+      <c r="K45" s="10">
+        <v>-75613329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>27</v>
       </c>
@@ -2176,8 +2402,14 @@
       <c r="I46" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="10">
+        <v>3261615</v>
+      </c>
+      <c r="K46" s="10">
+        <v>-76540823</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>65</v>
       </c>
@@ -2205,8 +2437,14 @@
       <c r="I47" s="3">
         <v>210</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="10">
+        <v>11637145</v>
+      </c>
+      <c r="K47" s="10">
+        <v>-72265589</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>43</v>
       </c>
@@ -2234,8 +2472,14 @@
       <c r="I48" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J48" s="10">
+        <v>9180754</v>
+      </c>
+      <c r="K48" s="10">
+        <v>-75914405</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>24</v>
       </c>
@@ -2263,8 +2507,14 @@
       <c r="I49" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J49" s="10">
+        <v>9240748</v>
+      </c>
+      <c r="K49" s="10">
+        <v>-74753151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
@@ -2292,8 +2542,14 @@
       <c r="I50" s="3">
         <v>1382</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="10">
+        <v>10343595</v>
+      </c>
+      <c r="K50" s="10">
+        <v>-74322237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>65</v>
       </c>
@@ -2321,8 +2577,14 @@
       <c r="I51" s="3">
         <v>1512</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="10">
+        <v>11378448</v>
+      </c>
+      <c r="K51" s="10">
+        <v>-72248203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>17</v>
       </c>
@@ -2350,8 +2612,14 @@
       <c r="I52" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="10">
+        <v>10856062</v>
+      </c>
+      <c r="K52" s="10">
+        <v>-74774442</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>30</v>
       </c>
@@ -2379,8 +2647,14 @@
       <c r="I53" s="3">
         <v>8695</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="10">
+        <v>5077517</v>
+      </c>
+      <c r="K53" s="10">
+        <v>-75516268</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>10</v>
       </c>
@@ -2408,8 +2682,14 @@
       <c r="I54" s="3">
         <v>7715</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="10">
+        <v>6255294</v>
+      </c>
+      <c r="K54" s="10">
+        <v>-75564904</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>72</v>
       </c>
@@ -2437,8 +2717,14 @@
       <c r="I55" s="3">
         <v>1676</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="10">
+        <v>3485893</v>
+      </c>
+      <c r="K55" s="10">
+        <v>-73116660</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>43</v>
       </c>
@@ -2466,8 +2752,14 @@
       <c r="I56" s="3">
         <v>2661</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="10">
+        <v>8623775</v>
+      </c>
+      <c r="K56" s="10">
+        <v>75970308</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>38</v>
       </c>
@@ -2495,8 +2787,14 @@
       <c r="I57" s="3">
         <v>4452</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="10">
+        <v>4678858</v>
+      </c>
+      <c r="K57" s="10">
+        <v>-74232826</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>61</v>
       </c>
@@ -2524,8 +2822,14 @@
       <c r="I58" s="3">
         <v>4904</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="10">
+        <v>2017503</v>
+      </c>
+      <c r="K58" s="10">
+        <v>-77954097</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>58</v>
       </c>
@@ -2553,8 +2857,14 @@
       <c r="I59" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J59" s="10">
+        <v>2949610</v>
+      </c>
+      <c r="K59" s="10">
+        <v>-75265950</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>44</v>
       </c>
@@ -2582,8 +2892,14 @@
       <c r="I60" s="3">
         <v>2148</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="10">
+        <v>8279882</v>
+      </c>
+      <c r="K60" s="10">
+        <v>-72935462</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>27</v>
       </c>
@@ -2611,8 +2927,14 @@
       <c r="I61" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="10">
+        <v>3536811</v>
+      </c>
+      <c r="K61" s="10">
+        <v>-76296627</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>61</v>
       </c>
@@ -2640,8 +2962,14 @@
       <c r="I62" s="3">
         <v>5688</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="10">
+        <v>1207519</v>
+      </c>
+      <c r="K62" s="10">
+        <v>-77285892</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>46</v>
       </c>
@@ -2669,8 +2997,14 @@
       <c r="I63" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J63" s="10">
+        <v>4796639</v>
+      </c>
+      <c r="K63" s="10">
+        <v>-75782788</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>18</v>
       </c>
@@ -2698,8 +3032,14 @@
       <c r="I64" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" s="10">
+        <v>6984593</v>
+      </c>
+      <c r="K64" s="10">
+        <v>-73021266</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>58</v>
       </c>
@@ -2727,8 +3067,14 @@
       <c r="I65" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" s="10">
+        <v>1849461</v>
+      </c>
+      <c r="K65" s="10">
+        <v>-76104193</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>36</v>
       </c>
@@ -2756,8 +3102,14 @@
       <c r="I66" s="3">
         <v>1573</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" s="10">
+        <v>2482825</v>
+      </c>
+      <c r="K66" s="10">
+        <v>-76604158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>82</v>
       </c>
@@ -2785,8 +3137,14 @@
       <c r="I67" s="3">
         <v>1058</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="K67" s="10">
+        <v>-76139419</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>40</v>
       </c>
@@ -2814,8 +3172,14 @@
       <c r="I68" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" s="10">
+        <v>5694608</v>
+      </c>
+      <c r="K68" s="10">
+        <v>-76650499</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>15</v>
       </c>
@@ -2843,8 +3207,14 @@
       <c r="I69" s="3">
         <v>2842</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="10">
+        <v>4482536</v>
+      </c>
+      <c r="K69" s="10">
+        <v>-75686416</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>65</v>
       </c>
@@ -2872,8 +3242,14 @@
       <c r="I70" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" s="10">
+        <v>11537384</v>
+      </c>
+      <c r="K70" s="10">
+        <v>-72917060</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>10</v>
       </c>
@@ -2901,8 +3277,14 @@
       <c r="I71" s="3">
         <v>2532</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" s="10">
+        <v>6145946</v>
+      </c>
+      <c r="K71" s="10">
+        <v>-75375429</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>46</v>
       </c>
@@ -2930,8 +3312,14 @@
       <c r="I72" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" s="10">
+        <v>5107868</v>
+      </c>
+      <c r="K72" s="10">
+        <v>-75982958</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>10</v>
       </c>
@@ -2959,8 +3347,14 @@
       <c r="I73" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" s="10">
+        <v>6149918</v>
+      </c>
+      <c r="K73" s="10">
+        <v>-75616863</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>43</v>
       </c>
@@ -2988,12 +3382,18 @@
       <c r="I74" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="J74" s="10">
+        <v>8830242</v>
+      </c>
+      <c r="K74" s="10">
+        <v>-75446646</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C75" s="3">
@@ -3017,8 +3417,14 @@
       <c r="I75" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J75" s="10">
+        <v>12576357</v>
+      </c>
+      <c r="K75" s="10">
+        <v>-79303789</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>41</v>
       </c>
@@ -3046,8 +3452,14 @@
       <c r="I76" s="3">
         <v>1714</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J76" s="10">
+        <v>11158977</v>
+      </c>
+      <c r="K76" s="10">
+        <v>-73934921</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>18</v>
       </c>
@@ -3075,8 +3487,14 @@
       <c r="I77" s="3">
         <v>2853</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" s="10">
+        <v>6815745</v>
+      </c>
+      <c r="K77" s="10">
+        <v>-73233824</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>91</v>
       </c>
@@ -3104,8 +3522,14 @@
       <c r="I78" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" s="10">
+        <v>9320156</v>
+      </c>
+      <c r="K78" s="10">
+        <v>-75436479</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>38</v>
       </c>
@@ -3133,8 +3557,14 @@
       <c r="I79" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J79" s="10">
+        <v>4581560</v>
+      </c>
+      <c r="K79" s="10">
+        <v>-74211804</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>25</v>
       </c>
@@ -3162,8 +3592,14 @@
       <c r="I80" s="3">
         <v>720</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="10">
+        <v>5717724</v>
+      </c>
+      <c r="K80" s="10">
+        <v>-72930567</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>17</v>
       </c>
@@ -3191,8 +3627,14 @@
       <c r="I81" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" s="10">
+        <v>10915492</v>
+      </c>
+      <c r="K81" s="10">
+        <v>-74796907</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>91</v>
       </c>
@@ -3220,8 +3662,14 @@
       <c r="I82" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" s="10">
+        <v>9308861</v>
+      </c>
+      <c r="K82" s="10">
+        <v>-75235223</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>59</v>
       </c>
@@ -3249,8 +3697,14 @@
       <c r="I83" s="3">
         <v>3053</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" s="10">
+        <v>4198023</v>
+      </c>
+      <c r="K83" s="10">
+        <v>-75181930</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>27</v>
       </c>
@@ -3278,8 +3732,14 @@
       <c r="I84" s="3">
         <v>661</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" s="10">
+        <v>4091237</v>
+      </c>
+      <c r="K84" s="10">
+        <v>-76195938</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>61</v>
       </c>
@@ -3307,8 +3767,14 @@
       <c r="I85" s="3">
         <v>1558</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" s="10">
+        <v>1783378</v>
+      </c>
+      <c r="K85" s="10">
+        <v>-78789646</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>25</v>
       </c>
@@ -3336,8 +3802,14 @@
       <c r="I86" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" s="10">
+        <v>5541685</v>
+      </c>
+      <c r="K86" s="10">
+        <v>-73355727</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>10</v>
       </c>
@@ -3365,8 +3837,14 @@
       <c r="I87" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" s="10">
+        <v>8132901</v>
+      </c>
+      <c r="K87" s="10">
+        <v>-76599093</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>65</v>
       </c>
@@ -3394,8 +3872,14 @@
       <c r="I88" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" s="10">
+        <v>11717000</v>
+      </c>
+      <c r="K88" s="10">
+        <v>-72265153</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>27</v>
       </c>
@@ -3423,8 +3907,14 @@
       <c r="I89" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J89" s="10">
+        <v>3832700</v>
+      </c>
+      <c r="K89" s="10">
+        <v>-76438807</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>37</v>
       </c>
@@ -3452,12 +3942,18 @@
       <c r="I90" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" s="10">
+        <v>10473042</v>
+      </c>
+      <c r="K90" s="10">
+        <v>-73256744</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B91" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C91" s="3">
@@ -3481,8 +3977,14 @@
       <c r="I91" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K91" s="10">
+        <v>-70589628</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>104</v>
       </c>
@@ -3510,8 +4012,14 @@
       <c r="I92" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J92" s="10">
+        <v>4895791</v>
+      </c>
+      <c r="K92" s="10">
+        <v>-69609599</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>72</v>
       </c>
@@ -3539,8 +4047,14 @@
       <c r="I93" s="3">
         <v>186</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" s="10">
+        <v>4089058</v>
+      </c>
+      <c r="K93" s="10">
+        <v>-73507620</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>35</v>
       </c>
@@ -3568,8 +4082,14 @@
       <c r="I94" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" s="10">
+        <v>5337666</v>
+      </c>
+      <c r="K94" s="10">
+        <v>-72397610</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>27</v>
       </c>
@@ -3597,8 +4117,14 @@
       <c r="I95" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" s="10">
+        <v>3542424</v>
+      </c>
+      <c r="K95" s="10">
+        <v>-76495542</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>38</v>
       </c>
@@ -3625,6 +4151,12 @@
       </c>
       <c r="I96" s="3">
         <v>1251</v>
+      </c>
+      <c r="J96" s="10">
+        <v>5035445</v>
+      </c>
+      <c r="K96" s="10">
+        <v>-74008690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>